<commit_message>
Criando o arquivo Excel
Criando o arquivo Excel, biblioteca openpyxl
</commit_message>
<xml_diff>
--- a/empresa_banco_dados.xlsx
+++ b/empresa_banco_dados.xlsx
@@ -448,7 +448,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>mss (chave)</t>
+          <t>nss (chave)</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -498,19 +498,22 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>1001</v>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nome1</t>
+          <t>João</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mnome1</t>
+          <t>Carlos</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Snome1</t>
+          <t>Silva</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -520,29 +523,41 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>yyyy-mm-dd</t>
-        </is>
+          <t>1990-05-15</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>3500</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Endereco1</t>
-        </is>
+          <t>Rua A, 123</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>5001</v>
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="n">
+        <v>1002</v>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nome2</t>
+          <t>Maria</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mnome2</t>
+          <t>José</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Snome2</t>
+          <t>Souza</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -552,13 +567,22 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>yyyy-mm-dd</t>
-        </is>
+          <t>1992-08-22</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>3200</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Endereco2</t>
-        </is>
+          <t>Rua B, 456</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" t="n">
+        <v>5002</v>
       </c>
     </row>
   </sheetData>
@@ -608,26 +632,44 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Departamento1</t>
-        </is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1001</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>yyyy-mm-dd</t>
+          <t>2020-01-10</t>
         </is>
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Departamento2</t>
-        </is>
+          <t>RH</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1002</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>yyyy-mm-dd</t>
+          <t>2021-02-15</t>
         </is>
       </c>
     </row>
@@ -673,9 +715,12 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>101</v>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Projeto1</t>
+          <t>Projeto A</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -683,17 +728,26 @@
           <t>Localizacao1</t>
         </is>
       </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
+      <c r="A3" t="n">
+        <v>102</v>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Projeto2</t>
+          <t>Projeto B</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>Localizacao2</t>
         </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -743,9 +797,12 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>1001</v>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nome_dependente1</t>
+          <t>Maria Silva</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -755,19 +812,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>yyyy-mm-dd</t>
+          <t>2015-07-20</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Tipo1</t>
+          <t>Filha</t>
         </is>
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="n">
+        <v>1002</v>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nome_dependente2</t>
+          <t>João Souza</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -777,12 +837,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>yyyy-mm-dd</t>
+          <t>2018-11-10</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Tipo2</t>
+          <t>Filho</t>
         </is>
       </c>
     </row>
@@ -822,8 +882,28 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
-    <row r="3"/>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="n">
+        <v>101</v>
+      </c>
+      <c r="C2" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="n">
+        <v>102</v>
+      </c>
+      <c r="C3" t="n">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -861,12 +941,18 @@
           <t>Localizacao1</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
           <t>Localizacao2</t>
         </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>